<commit_message>
not resetting data bug fix
</commit_message>
<xml_diff>
--- a/savefile.xlsx
+++ b/savefile.xlsx
@@ -397,7 +397,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BF100"/>
+  <dimension ref="A1:BK100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
@@ -641,6 +641,22 @@
           <t>S-CTL4-1_0008.jpg</t>
         </is>
       </c>
+      <c r="BG1" t="n">
+        <v>3092.319768143945</v>
+      </c>
+      <c r="BH1" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
+      <c r="BI1" t="n">
+        <v>3370.667793744718</v>
+      </c>
+      <c r="BJ1" t="inlineStr">
+        <is>
+          <t>CK2_2_0006.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -827,6 +843,14 @@
           <t>S-CTL4-1_0008.jpg</t>
         </is>
       </c>
+      <c r="BG2" t="n">
+        <v>2892.766574085256</v>
+      </c>
+      <c r="BH2" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -949,6 +973,14 @@
           <t>S-CTL4-1_0008.jpg</t>
         </is>
       </c>
+      <c r="BG3" t="n">
+        <v>1382.381354908828</v>
+      </c>
+      <c r="BH3" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -1055,6 +1087,14 @@
           <t>S-CTL4-1_0008.jpg</t>
         </is>
       </c>
+      <c r="BG4" t="n">
+        <v>1585.859195749306</v>
+      </c>
+      <c r="BH4" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -1161,6 +1201,14 @@
           <t>S-CTL4-1_0008.jpg</t>
         </is>
       </c>
+      <c r="BG5" t="n">
+        <v>3071.48895060983</v>
+      </c>
+      <c r="BH5" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1259,6 +1307,14 @@
           <t>S-CTL4-1_0008.jpg</t>
         </is>
       </c>
+      <c r="BG6" t="n">
+        <v>705.2288370969691</v>
+      </c>
+      <c r="BH6" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1349,6 +1405,14 @@
           <t>S-CTL4-1_0008.jpg</t>
         </is>
       </c>
+      <c r="BG7" t="n">
+        <v>1756.430382804009</v>
+      </c>
+      <c r="BH7" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1439,6 +1503,14 @@
           <t>S-CTL4-1_0008.jpg</t>
         </is>
       </c>
+      <c r="BG8" t="n">
+        <v>2316.447288974762</v>
+      </c>
+      <c r="BH8" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="AC9" t="n">
@@ -1521,6 +1593,14 @@
           <t>S-CTL4-1_0008.jpg</t>
         </is>
       </c>
+      <c r="BG9" t="n">
+        <v>774.9667914503081</v>
+      </c>
+      <c r="BH9" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="AC10" t="n">
@@ -1603,6 +1683,14 @@
           <t>S-CTL4-1_0008.jpg</t>
         </is>
       </c>
+      <c r="BG10" t="n">
+        <v>1857.565511411666</v>
+      </c>
+      <c r="BH10" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="AC11" t="n">
@@ -1685,6 +1773,14 @@
           <t>S-CTL4-1_0008.jpg</t>
         </is>
       </c>
+      <c r="BG11" t="n">
+        <v>3432.254558628186</v>
+      </c>
+      <c r="BH11" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="AC12" t="n">
@@ -1767,6 +1863,14 @@
           <t>S-CTL4-1_0008.jpg</t>
         </is>
       </c>
+      <c r="BG12" t="n">
+        <v>1322.304069556817</v>
+      </c>
+      <c r="BH12" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="AC13" t="n">
@@ -1849,6 +1953,14 @@
           <t>S-CTL4-1_0008.jpg</t>
         </is>
       </c>
+      <c r="BG13" t="n">
+        <v>2103.308779132955</v>
+      </c>
+      <c r="BH13" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="AC14" t="n">
@@ -1931,6 +2043,14 @@
           <t>S-CTL4-1_0008.jpg</t>
         </is>
       </c>
+      <c r="BG14" t="n">
+        <v>1784.50670208912</v>
+      </c>
+      <c r="BH14" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="AC15" t="n">
@@ -2013,6 +2133,14 @@
           <t>S-CTL4-1_0008.jpg</t>
         </is>
       </c>
+      <c r="BG15" t="n">
+        <v>3243.2677212897</v>
+      </c>
+      <c r="BH15" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="AC16" t="n">
@@ -2095,6 +2223,14 @@
           <t>S-CTL4-1_0008.jpg</t>
         </is>
       </c>
+      <c r="BG16" t="n">
+        <v>1555.669605120155</v>
+      </c>
+      <c r="BH16" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="AC17" t="n">
@@ -2177,6 +2313,14 @@
           <t>S-CTL4-1_0008.jpg</t>
         </is>
       </c>
+      <c r="BG17" t="n">
+        <v>2628.305760173892</v>
+      </c>
+      <c r="BH17" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="AC18" t="n">
@@ -2259,6 +2403,14 @@
           <t>S-CTL4-1_0008.jpg</t>
         </is>
       </c>
+      <c r="BG18" t="n">
+        <v>2736.082598719962</v>
+      </c>
+      <c r="BH18" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="AC19" t="n">
@@ -2341,6 +2493,14 @@
           <t>S-CTL4-1_0008.jpg</t>
         </is>
       </c>
+      <c r="BG19" t="n">
+        <v>2841.142374109408</v>
+      </c>
+      <c r="BH19" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="AC20" t="n">
@@ -2423,6 +2583,14 @@
           <t>S-CTL4-1_0008.jpg</t>
         </is>
       </c>
+      <c r="BG20" t="n">
+        <v>2453.508030431108</v>
+      </c>
+      <c r="BH20" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="AC21" t="n">
@@ -2497,6 +2665,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG21" t="n">
+        <v>2108.441009539911</v>
+      </c>
+      <c r="BH21" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="AC22" t="n">
@@ -2571,6 +2747,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG22" t="n">
+        <v>1711.145996860283</v>
+      </c>
+      <c r="BH22" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="AC23" t="n">
@@ -2645,6 +2829,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG23" t="n">
+        <v>1949.643762830576</v>
+      </c>
+      <c r="BH23" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="AC24" t="n">
@@ -2719,6 +2911,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG24" t="n">
+        <v>2670.571187054704</v>
+      </c>
+      <c r="BH24" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="AC25" t="n">
@@ -2793,6 +2993,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG25" t="n">
+        <v>2157.951938171719</v>
+      </c>
+      <c r="BH25" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="AC26" t="n">
@@ -2867,6 +3075,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG26" t="n">
+        <v>1914.32194179447</v>
+      </c>
+      <c r="BH26" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="AC27" t="n">
@@ -2941,6 +3157,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG27" t="n">
+        <v>1059.654631083203</v>
+      </c>
+      <c r="BH27" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="AC28" t="n">
@@ -3015,6 +3239,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG28" t="n">
+        <v>1575.292839029103</v>
+      </c>
+      <c r="BH28" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="AC29" t="n">
@@ -3089,6 +3321,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG29" t="n">
+        <v>996.2564907619854</v>
+      </c>
+      <c r="BH29" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="AC30" t="n">
@@ -3163,6 +3403,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG30" t="n">
+        <v>1583.444028498974</v>
+      </c>
+      <c r="BH30" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="AC31" t="n">
@@ -3237,6 +3485,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG31" t="n">
+        <v>2029.646177997827</v>
+      </c>
+      <c r="BH31" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="AC32" t="n">
@@ -3311,6 +3567,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG32" t="n">
+        <v>2214.708368554523</v>
+      </c>
+      <c r="BH32" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="AC33" t="n">
@@ -3385,6 +3649,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG33" t="n">
+        <v>714.2857142857144</v>
+      </c>
+      <c r="BH33" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="AC34" t="n">
@@ -3459,6 +3731,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG34" t="n">
+        <v>1993.418669242845</v>
+      </c>
+      <c r="BH34" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="AC35" t="n">
@@ -3533,6 +3813,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG35" t="n">
+        <v>1809.865958217607</v>
+      </c>
+      <c r="BH35" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="AC36" t="n">
@@ -3607,6 +3895,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG36" t="n">
+        <v>1664.65402729139</v>
+      </c>
+      <c r="BH36" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="AC37" t="n">
@@ -3681,6 +3977,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG37" t="n">
+        <v>979.9541118222439</v>
+      </c>
+      <c r="BH37" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="AC38" t="n">
@@ -3755,6 +4059,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG38" t="n">
+        <v>1676.126071730468</v>
+      </c>
+      <c r="BH38" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="AC39" t="n">
@@ -3829,6 +4141,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG39" t="n">
+        <v>665.6804733727812</v>
+      </c>
+      <c r="BH39" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="AC40" t="n">
@@ -3903,6 +4223,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG40" t="n">
+        <v>1151.732882502114</v>
+      </c>
+      <c r="BH40" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="AC41" t="n">
@@ -3977,6 +4305,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG41" t="n">
+        <v>942.8209153483881</v>
+      </c>
+      <c r="BH41" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="AC42" t="n">
@@ -4051,6 +4387,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG42" t="n">
+        <v>1076.862697741819</v>
+      </c>
+      <c r="BH42" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="AC43" t="n">
@@ -4125,6 +4469,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG43" t="n">
+        <v>1165.620094191523</v>
+      </c>
+      <c r="BH43" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="AC44" t="n">
@@ -4199,6 +4551,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG44" t="n">
+        <v>935.5754135973918</v>
+      </c>
+      <c r="BH44" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="AC45" t="n">
@@ -4273,6 +4633,14 @@
           <t>S-CTL4-1_1.jpg</t>
         </is>
       </c>
+      <c r="BG45" t="n">
+        <v>1112.788310590509</v>
+      </c>
+      <c r="BH45" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="AC46" t="n">
@@ -4339,6 +4707,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG46" t="n">
+        <v>2262.407921748581</v>
+      </c>
+      <c r="BH46" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="AC47" t="n">
@@ -4405,6 +4781,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG47" t="n">
+        <v>1936.058447047458</v>
+      </c>
+      <c r="BH47" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="AC48" t="n">
@@ -4471,6 +4855,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG48" t="n">
+        <v>1610.61466006521</v>
+      </c>
+      <c r="BH48" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="AC49" t="n">
@@ -4537,6 +4929,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG49" t="n">
+        <v>1539.065330274122</v>
+      </c>
+      <c r="BH49" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="AC50" t="n">
@@ -4603,6 +5003,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG50" t="n">
+        <v>2127.762347542568</v>
+      </c>
+      <c r="BH50" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="AC51" t="n">
@@ -4669,6 +5077,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG51" t="n">
+        <v>3037.978505011473</v>
+      </c>
+      <c r="BH51" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="AC52" t="n">
@@ -4735,6 +5151,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG52" t="n">
+        <v>1372.7206859075</v>
+      </c>
+      <c r="BH52" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="AC53" t="n">
@@ -4801,6 +5225,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG53" t="n">
+        <v>1259.509721048183</v>
+      </c>
+      <c r="BH53" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="AC54" t="n">
@@ -4867,6 +5299,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG54" t="n">
+        <v>2652.457432677214</v>
+      </c>
+      <c r="BH54" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="AC55" t="n">
@@ -4933,6 +5373,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG55" t="n">
+        <v>1091.353701243811</v>
+      </c>
+      <c r="BH55" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="AC56" t="n">
@@ -4999,6 +5447,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG56" t="n">
+        <v>1691.220867045043</v>
+      </c>
+      <c r="BH56" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="AC57" t="n">
@@ -5065,6 +5521,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG57" t="n">
+        <v>1678.843134887091</v>
+      </c>
+      <c r="BH57" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="AC58" t="n">
@@ -5131,6 +5595,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG58" t="n">
+        <v>971.8029223523731</v>
+      </c>
+      <c r="BH58" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="AC59" t="n">
@@ -5197,6 +5669,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG59" t="n">
+        <v>734.5127400072456</v>
+      </c>
+      <c r="BH59" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="AC60" t="n">
@@ -5263,6 +5743,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG60" t="n">
+        <v>2896.691220867046</v>
+      </c>
+      <c r="BH60" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="AC61" t="n">
@@ -5329,6 +5817,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG61" t="n">
+        <v>787.34452360826</v>
+      </c>
+      <c r="BH61" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="AC62" t="n">
@@ -5395,6 +5891,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG62" t="n">
+        <v>735.7203236324117</v>
+      </c>
+      <c r="BH62" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="AC63" t="n">
@@ -5461,6 +5965,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG63" t="n">
+        <v>2321.579519381718</v>
+      </c>
+      <c r="BH63" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="AC64" t="n">
@@ -5527,6 +6039,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG64" t="n">
+        <v>1222.678420480619</v>
+      </c>
+      <c r="BH64" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="AC65" t="n">
@@ -5593,6 +6113,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG65" t="n">
+        <v>1764.883468180172</v>
+      </c>
+      <c r="BH65" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="AC66" t="n">
@@ -5659,6 +6187,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG66" t="n">
+        <v>2736.988286438836</v>
+      </c>
+      <c r="BH66" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="AC67" t="n">
@@ -5725,6 +6261,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG67" t="n">
+        <v>2444.451153242363</v>
+      </c>
+      <c r="BH67" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="AC68" t="n">
@@ -5791,6 +6335,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG68" t="n">
+        <v>1727.146479893733</v>
+      </c>
+      <c r="BH68" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="AC69" t="n">
@@ -5857,6 +6409,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG69" t="n">
+        <v>717.3046733486295</v>
+      </c>
+      <c r="BH69" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="AC70" t="n">
@@ -5923,6 +6483,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG70" t="n">
+        <v>899.0460089361191</v>
+      </c>
+      <c r="BH70" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="AC71" t="n">
@@ -5989,6 +6557,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG71" t="n">
+        <v>1623.898079942036</v>
+      </c>
+      <c r="BH71" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="AC72" t="n">
@@ -6055,6 +6631,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG72" t="n">
+        <v>2033.872720685908</v>
+      </c>
+      <c r="BH72" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="AC73" t="n">
@@ -6113,6 +6697,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG73" t="n">
+        <v>1065.390653302741</v>
+      </c>
+      <c r="BH73" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="AC74" t="n">
@@ -6163,6 +6755,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG74" t="n">
+        <v>1504.347301050598</v>
+      </c>
+      <c r="BH74" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="AC75" t="n">
@@ -6213,6 +6813,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG75" t="n">
+        <v>992.0299480739043</v>
+      </c>
+      <c r="BH75" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="AC76" t="n">
@@ -6263,6 +6871,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG76" t="n">
+        <v>930.7450790967276</v>
+      </c>
+      <c r="BH76" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="AC77" t="n">
@@ -6313,6 +6929,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG77" t="n">
+        <v>704.9269411906776</v>
+      </c>
+      <c r="BH77" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="AI78" t="n">
@@ -6355,6 +6979,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG78" t="n">
+        <v>1319.285110493902</v>
+      </c>
+      <c r="BH78" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="AI79" t="n">
@@ -6397,6 +7029,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG79" t="n">
+        <v>922.8957855331483</v>
+      </c>
+      <c r="BH79" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="AQ80" t="n">
@@ -6423,6 +7063,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG80" t="n">
+        <v>791.5710662963412</v>
+      </c>
+      <c r="BH80" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="AQ81" t="n">
@@ -6449,6 +7097,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG81" t="n">
+        <v>950.3683130056759</v>
+      </c>
+      <c r="BH81" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="AQ82" t="n">
@@ -6475,6 +7131,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG82" t="n">
+        <v>1115.203477840841</v>
+      </c>
+      <c r="BH82" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="AQ83" t="n">
@@ -6501,6 +7165,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG83" t="n">
+        <v>594.1311435816932</v>
+      </c>
+      <c r="BH83" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="AQ84" t="n">
@@ -6527,6 +7199,14 @@
           <t>S-CTL4-2_0009.jpg</t>
         </is>
       </c>
+      <c r="BG84" t="n">
+        <v>655.1141166525783</v>
+      </c>
+      <c r="BH84" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="AQ85" t="n">
@@ -6551,6 +7231,14 @@
       <c r="AZ85" t="inlineStr">
         <is>
           <t>S-CTL4-2_0009.jpg</t>
+        </is>
+      </c>
+      <c r="BG85" t="n">
+        <v>1259.811616954474</v>
+      </c>
+      <c r="BH85" t="inlineStr">
+        <is>
+          <t>S-CTL4-1_0008.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>